<commit_message>
added google scripts to order repository
</commit_message>
<xml_diff>
--- a/orderflex/src/App/FellAppBundle/Util/GoogleForm/FellowshipRecommendationLetters/BackupSpreadsheet.xlsx
+++ b/orderflex/src/App/FellAppBundle/Util/GoogleForm/FellowshipRecommendationLetters/BackupSpreadsheet.xlsx
@@ -226,18 +226,18 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="75.43"/>
-    <col customWidth="1" min="2" max="6" width="21.57"/>
-    <col customWidth="1" min="7" max="7" width="32.43"/>
-    <col customWidth="1" min="8" max="16" width="21.57"/>
-    <col customWidth="1" min="17" max="17" width="19.0"/>
-    <col customWidth="1" min="18" max="18" width="21.14"/>
-    <col customWidth="1" min="19" max="19" width="24.14"/>
-    <col customWidth="1" min="20" max="20" width="24.57"/>
-    <col customWidth="1" min="21" max="21" width="21.57"/>
-    <col customWidth="1" min="22" max="23" width="28.71"/>
+    <col customWidth="1" min="1" max="1" width="66.0"/>
+    <col customWidth="1" min="2" max="6" width="18.88"/>
+    <col customWidth="1" min="7" max="7" width="28.38"/>
+    <col customWidth="1" min="8" max="16" width="18.88"/>
+    <col customWidth="1" min="17" max="17" width="16.63"/>
+    <col customWidth="1" min="18" max="18" width="18.5"/>
+    <col customWidth="1" min="19" max="19" width="21.13"/>
+    <col customWidth="1" min="20" max="20" width="21.5"/>
+    <col customWidth="1" min="21" max="21" width="18.88"/>
+    <col customWidth="1" min="22" max="23" width="25.13"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>